<commit_message>
MonsterTable 에 boss|Bool 컬럼 추가
</commit_message>
<xml_diff>
--- a/Excel/Stage.xlsx
+++ b/Excel/Stage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectNoname\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1857F6C1-9139-4F4C-B07E-36A1927B4915}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2A4CA20-9E73-4102-B6FD-D5423D318306}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{566BA174-F383-48D7-A97F-7F70BBC36EC1}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{566BA174-F383-48D7-A97F-7F70BBC36EC1}"/>
   </bookViews>
   <sheets>
     <sheet name="StageTable" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="859" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="860" uniqueCount="62">
   <si>
     <t>multiHp|Float</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -224,6 +224,10 @@
   </si>
   <si>
     <t>Wall_24_24_3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>boss|Bool</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -20152,7 +20156,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{793CE6DE-869E-4A11-BDAA-E54547146D5F}">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
@@ -20482,16 +20486,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDB0DF-5C8E-46E0-A66A-0B4AF86ECDFD}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -20510,8 +20514,11 @@
       <c r="F1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -20530,8 +20537,11 @@
       <c r="F2">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -20550,8 +20560,11 @@
       <c r="F3">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -20569,6 +20582,9 @@
       </c>
       <c r="F4">
         <v>2</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
StageTable 에 bossHpRatioPer1Line 컬럼 추가
</commit_message>
<xml_diff>
--- a/Excel/Stage.xlsx
+++ b/Excel/Stage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectNoname\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5FBD232-F155-4043-A7DA-D699E266907E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB1DA7CF-911E-4784-9DFD-9FD3F97CED80}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{566BA174-F383-48D7-A97F-7F70BBC36EC1}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{566BA174-F383-48D7-A97F-7F70BBC36EC1}"/>
   </bookViews>
   <sheets>
     <sheet name="StageTable" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="861" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="862" uniqueCount="63">
   <si>
     <t>multiHp|Float</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -229,6 +229,10 @@
   </si>
   <si>
     <t>MadcapBoss</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bossHpRatioPer1Line|Float</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -593,9 +597,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD089199-7F78-438F-98D3-F9F9DD953178}">
-  <dimension ref="A1:J751"/>
+  <dimension ref="A1:K751"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
@@ -611,7 +615,7 @@
     <col min="9" max="10" width="21.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -642,8 +646,11 @@
       <c r="J1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -672,7 +679,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -698,7 +705,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -724,7 +731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -750,7 +757,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1</v>
       </c>
@@ -776,7 +783,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1</v>
       </c>
@@ -802,7 +809,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1</v>
       </c>
@@ -828,7 +835,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1</v>
       </c>
@@ -854,7 +861,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1</v>
       </c>
@@ -880,7 +887,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1</v>
       </c>
@@ -905,8 +912,11 @@
       <c r="I11" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>1</v>
       </c>
@@ -932,7 +942,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>1</v>
       </c>
@@ -958,7 +968,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>1</v>
       </c>
@@ -984,7 +994,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>1</v>
       </c>
@@ -1010,7 +1020,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>1</v>
       </c>
@@ -1036,7 +1046,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>1</v>
       </c>
@@ -1062,7 +1072,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>1</v>
       </c>
@@ -1088,7 +1098,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>1</v>
       </c>
@@ -1114,7 +1124,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>1</v>
       </c>
@@ -1140,7 +1150,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>1</v>
       </c>
@@ -1165,8 +1175,11 @@
       <c r="I21" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>1</v>
       </c>
@@ -1192,7 +1205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>1</v>
       </c>
@@ -1218,7 +1231,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>1</v>
       </c>
@@ -1244,7 +1257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>1</v>
       </c>
@@ -1270,7 +1283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>1</v>
       </c>
@@ -1296,7 +1309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>1</v>
       </c>
@@ -1322,7 +1335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>1</v>
       </c>
@@ -1348,7 +1361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>1</v>
       </c>
@@ -1374,7 +1387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>1</v>
       </c>
@@ -1400,7 +1413,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>1</v>
       </c>
@@ -1426,7 +1439,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>1</v>
       </c>
@@ -20489,7 +20502,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDB0DF-5C8E-46E0-A66A-0B4AF86ECDFD}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>

<commit_message>
MonsterTable 에 evadeRate 컬럼 추가
</commit_message>
<xml_diff>
--- a/Excel/Stage.xlsx
+++ b/Excel/Stage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectNoname\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F67C92B1-4F94-4944-8504-6A02ADD12A2B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CE4F727-E07C-4FFE-8985-ECBEA6F3EF1C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{566BA174-F383-48D7-A97F-7F70BBC36EC1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{566BA174-F383-48D7-A97F-7F70BBC36EC1}"/>
   </bookViews>
   <sheets>
     <sheet name="StageTable" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1690" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1691" uniqueCount="79">
   <si>
     <t>chapter|Int</t>
   </si>
@@ -273,6 +273,10 @@
     <t>passiveAffectorValueId|String!</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>evadeRate|Float</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -325,12 +329,7 @@
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.14996795556505021"/>
-      </font>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color theme="0" tint="-0.14996795556505021"/>
@@ -25844,17 +25843,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDB0DF-5C8E-46E0-A66A-0B4AF86ECDFD}">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.375" customWidth="1"/>
-    <col min="11" max="11" width="26.75" customWidth="1"/>
+    <col min="12" max="12" width="26.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>38</v>
       </c>
@@ -25874,22 +25873,25 @@
         <v>43</v>
       </c>
       <c r="G1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H1" t="s">
         <v>44</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>52</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>50</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>45</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>46</v>
       </c>
@@ -25908,20 +25910,23 @@
       <c r="F2">
         <v>3</v>
       </c>
-      <c r="G2" t="b">
+      <c r="G2">
         <v>0</v>
       </c>
       <c r="H2" t="b">
-        <v>1</v>
-      </c>
-      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="I2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J2">
         <v>1003</v>
       </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>47</v>
       </c>
@@ -25940,17 +25945,20 @@
       <c r="F3">
         <v>2.5</v>
       </c>
-      <c r="G3" t="b">
-        <v>0</v>
+      <c r="G3">
+        <v>0.9</v>
       </c>
       <c r="H3" t="b">
-        <v>1</v>
-      </c>
-      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="I3" t="b">
+        <v>1</v>
+      </c>
+      <c r="K3">
         <v>10.8</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>48</v>
       </c>
@@ -25969,14 +25977,17 @@
       <c r="F4">
         <v>2</v>
       </c>
-      <c r="G4" t="b">
+      <c r="G4">
         <v>0</v>
       </c>
       <c r="H4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="I4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>49</v>
       </c>
@@ -25995,20 +26006,23 @@
       <c r="F5">
         <v>2.5</v>
       </c>
-      <c r="G5" t="b">
-        <v>1</v>
+      <c r="G5">
+        <v>0</v>
       </c>
       <c r="H5" t="b">
         <v>1</v>
       </c>
-      <c r="I5">
+      <c r="I5" t="b">
+        <v>1</v>
+      </c>
+      <c r="J5">
         <v>1002</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>76</v>
       </c>
@@ -26027,21 +26041,24 @@
       <c r="F6">
         <v>1.8</v>
       </c>
-      <c r="G6" t="b">
-        <v>0</v>
+      <c r="G6">
+        <v>0.2</v>
       </c>
       <c r="H6" t="b">
-        <v>1</v>
-      </c>
-      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="I6" t="b">
+        <v>1</v>
+      </c>
+      <c r="K6">
         <v>10.8</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="K1">
+  <conditionalFormatting sqref="L1">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>K1=K1048554</formula>
+      <formula>L1=L1048554</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
MapTable 에 portalFlag 컬럼 추가
</commit_message>
<xml_diff>
--- a/Excel/Stage.xlsx
+++ b/Excel/Stage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectNoname\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE09E9E3-B5CB-49E6-A6ED-EEA8AB9EC121}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D83D989-9B11-416D-A024-73E43938BC74}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{566BA174-F383-48D7-A97F-7F70BBC36EC1}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{566BA174-F383-48D7-A97F-7F70BBC36EC1}"/>
   </bookViews>
   <sheets>
     <sheet name="StageTable" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1693" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1716" uniqueCount="84">
   <si>
     <t>chapter|Int</t>
   </si>
@@ -283,6 +283,18 @@
   </si>
   <si>
     <t>CallInvincibleTortoise</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>portalFlag|String</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PortalFlag_0_Empty</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PortalFlag_12_40_1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -25438,18 +25450,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{793CE6DE-869E-4A11-BDAA-E54547146D5F}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="23.625" customWidth="1"/>
-    <col min="6" max="6" width="21.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="23.625" customWidth="1"/>
+    <col min="7" max="7" width="21.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>29</v>
       </c>
@@ -25466,10 +25478,13 @@
         <v>32</v>
       </c>
       <c r="F1" t="s">
+        <v>81</v>
+      </c>
+      <c r="G1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>64</v>
       </c>
@@ -25485,8 +25500,11 @@
       <c r="E2" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -25502,8 +25520,11 @@
       <c r="E3" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -25519,8 +25540,11 @@
       <c r="E4" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -25536,8 +25560,11 @@
       <c r="E5" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -25553,8 +25580,11 @@
       <c r="E6" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -25570,8 +25600,11 @@
       <c r="E7" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -25587,8 +25620,11 @@
       <c r="E8" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F8" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -25604,8 +25640,11 @@
       <c r="E9" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -25621,8 +25660,11 @@
       <c r="E10" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F10" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -25638,8 +25680,11 @@
       <c r="E11" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F11" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -25655,8 +25700,11 @@
       <c r="E12" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F12" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -25672,8 +25720,11 @@
       <c r="E13" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F13" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -25689,8 +25740,11 @@
       <c r="E14" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F14" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -25706,8 +25760,11 @@
       <c r="E15" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F15" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -25723,8 +25780,11 @@
       <c r="E16" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F16" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -25740,8 +25800,11 @@
       <c r="E17" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F17" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>26</v>
       </c>
@@ -25757,8 +25820,11 @@
       <c r="E18" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F18" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -25774,8 +25840,11 @@
       <c r="E19" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F19" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -25791,8 +25860,11 @@
       <c r="E20" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F20" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>28</v>
       </c>
@@ -25808,8 +25880,11 @@
       <c r="E21" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F21" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>13</v>
       </c>
@@ -25825,8 +25900,11 @@
       <c r="E22" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F22" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -25841,6 +25919,9 @@
       </c>
       <c r="E23" t="s">
         <v>72</v>
+      </c>
+      <c r="F23" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -25853,7 +25934,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDB0DF-5C8E-46E0-A66A-0B4AF86ECDFD}">
   <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>

<commit_message>
MapTable 에 mirrorOffset 컬럼 추가
</commit_message>
<xml_diff>
--- a/Excel/Stage.xlsx
+++ b/Excel/Stage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectNoname\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F53D04EF-3653-4FAB-9611-5AE0D5BBFB3E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{402141E7-5DD1-4864-A645-D9975FE80889}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{566BA174-F383-48D7-A97F-7F70BBC36EC1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4329" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4330" uniqueCount="371">
   <si>
     <t>chapter|Int</t>
   </si>
@@ -1156,6 +1156,10 @@
   <si>
     <t>Actor001, Actor004</t>
   </si>
+  <si>
+    <t>mirrorOffset|Float</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -87593,21 +87597,23 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{793CE6DE-869E-4A11-BDAA-E54547146D5F}">
-  <dimension ref="A1:J60"/>
+  <dimension ref="A1:K60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="H54" sqref="H54"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.5" bestFit="1" customWidth="1"/>
     <col min="2" max="6" width="23.625" customWidth="1"/>
     <col min="7" max="7" width="21.375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.375" customWidth="1"/>
-    <col min="9" max="9" width="18" customWidth="1"/>
-    <col min="10" max="10" width="21.375" customWidth="1"/>
+    <col min="8" max="9" width="21.375" customWidth="1"/>
+    <col min="10" max="10" width="18" customWidth="1"/>
+    <col min="11" max="11" width="21.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -87630,16 +87636,19 @@
         <v>78</v>
       </c>
       <c r="H1" t="s">
+        <v>370</v>
+      </c>
+      <c r="I1" t="s">
         <v>126</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>102</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>59</v>
       </c>
@@ -87659,7 +87668,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -87679,7 +87688,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -87699,7 +87708,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -87719,7 +87728,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -87739,7 +87748,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -87759,7 +87768,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -87779,7 +87788,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -87799,7 +87808,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -87819,7 +87828,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>230</v>
       </c>
@@ -87839,7 +87848,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -87859,7 +87868,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -87879,7 +87888,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -87899,7 +87908,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>243</v>
       </c>
@@ -87919,7 +87928,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -88579,7 +88588,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>276</v>
       </c>
@@ -88599,7 +88608,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>277</v>
       </c>
@@ -88619,7 +88628,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>17</v>
       </c>
@@ -88642,7 +88651,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>27</v>
       </c>
@@ -88665,7 +88674,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>255</v>
       </c>
@@ -88687,17 +88696,20 @@
       <c r="G53" t="s">
         <v>362</v>
       </c>
-      <c r="H53" t="s">
+      <c r="H53">
+        <v>75</v>
+      </c>
+      <c r="I53" t="s">
         <v>363</v>
       </c>
-      <c r="I53" t="s">
+      <c r="J53" t="s">
         <v>364</v>
       </c>
-      <c r="J53" t="s">
+      <c r="K53" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>268</v>
       </c>
@@ -88719,17 +88731,20 @@
       <c r="G54" t="s">
         <v>366</v>
       </c>
-      <c r="H54" t="s">
+      <c r="H54">
+        <v>50</v>
+      </c>
+      <c r="I54" t="s">
         <v>367</v>
       </c>
-      <c r="I54" t="s">
+      <c r="J54" t="s">
         <v>368</v>
       </c>
-      <c r="J54" t="s">
+      <c r="K54" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>278</v>
       </c>
@@ -88752,7 +88767,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>12</v>
       </c>
@@ -88772,7 +88787,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>22</v>
       </c>
@@ -88792,7 +88807,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>250</v>
       </c>
@@ -88812,7 +88827,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>262</v>
       </c>
@@ -88832,7 +88847,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>273</v>
       </c>

</xml_diff>

<commit_message>
노아머 HP 배율 1 => 1.25
</commit_message>
<xml_diff>
--- a/Excel/Stage.xlsx
+++ b/Excel/Stage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectNoname\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89851762-5ED2-440A-A3B3-E38A239414B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCEEA84D-318A-4707-984A-45EDEBFD4483}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{566BA174-F383-48D7-A97F-7F70BBC36EC1}"/>
   </bookViews>
@@ -94317,7 +94317,7 @@
         <v>193</v>
       </c>
       <c r="B35">
-        <v>1</v>
+        <v>1.25</v>
       </c>
       <c r="C35">
         <v>1.1000000000000001</v>

</xml_diff>

<commit_message>
Hermit 공격력 0.7 이속 0.8 터렛 HP 1.5 => 1.2 목닥 이속 1.25 => 1
</commit_message>
<xml_diff>
--- a/Excel/Stage.xlsx
+++ b/Excel/Stage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectNoname\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77EAD15C-481B-4088-A451-F0A3CE92A548}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00C03AA9-17C7-4694-98C5-7C589497EFC4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{566BA174-F383-48D7-A97F-7F70BBC36EC1}"/>
   </bookViews>
@@ -67315,7 +67315,7 @@
         <v>0.3</v>
       </c>
       <c r="C57">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="D57">
         <v>0.66666666699999999</v>
@@ -67324,7 +67324,7 @@
         <v>2</v>
       </c>
       <c r="F57">
-        <v>1.25</v>
+        <v>0.8</v>
       </c>
       <c r="G57">
         <v>0</v>
@@ -67350,7 +67350,7 @@
         <v>1320</v>
       </c>
       <c r="B58">
-        <v>1.5</v>
+        <v>1.2</v>
       </c>
       <c r="C58">
         <v>0.8</v>
@@ -67388,7 +67388,7 @@
         <v>1321</v>
       </c>
       <c r="B59">
-        <v>1.5</v>
+        <v>1.2</v>
       </c>
       <c r="C59">
         <v>0.8</v>
@@ -67473,7 +67473,7 @@
         <v>2</v>
       </c>
       <c r="F61">
-        <v>1.25</v>
+        <v>1</v>
       </c>
       <c r="G61">
         <v>0</v>

</xml_diff>

<commit_message>
FairyFlower SpiderGreen 테이블 추가
</commit_message>
<xml_diff>
--- a/Excel/Stage.xlsx
+++ b/Excel/Stage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectNoname\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEC44288-B9D1-4CE5-8978-9888C57E2E1C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF4322A9-297C-4BAF-84B0-6B21201A7407}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{566BA174-F383-48D7-A97F-7F70BBC36EC1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{566BA174-F383-48D7-A97F-7F70BBC36EC1}"/>
   </bookViews>
   <sheets>
     <sheet name="ChapterTable" sheetId="5" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6048" uniqueCount="2440">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6050" uniqueCount="2442">
   <si>
     <t>chapter|Int</t>
   </si>
@@ -7357,6 +7357,12 @@
   </si>
   <si>
     <t>Deadweight</t>
+  </si>
+  <si>
+    <t>FairyFlower</t>
+  </si>
+  <si>
+    <t>SpiderGreen</t>
   </si>
 </sst>
 </file>
@@ -77724,7 +77730,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDB0DF-5C8E-46E0-A66A-0B4AF86ECDFD}">
-  <dimension ref="A1:N144"/>
+  <dimension ref="A1:N146"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -80268,7 +80274,7 @@
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>2439</v>
+        <v>2440</v>
       </c>
       <c r="B72">
         <v>1</v>
@@ -80303,7 +80309,7 @@
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>1038</v>
+        <v>2441</v>
       </c>
       <c r="B73">
         <v>1</v>
@@ -80338,7 +80344,7 @@
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>65</v>
+        <v>2439</v>
       </c>
       <c r="B74">
         <v>1</v>
@@ -80353,7 +80359,7 @@
         <v>2</v>
       </c>
       <c r="F74">
-        <v>0.7</v>
+        <v>1.25</v>
       </c>
       <c r="G74">
         <v>0</v>
@@ -80367,16 +80373,13 @@
       <c r="K74">
         <v>10</v>
       </c>
-      <c r="L74" t="s">
-        <v>66</v>
-      </c>
       <c r="M74">
         <v>1</v>
       </c>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>59</v>
+        <v>1038</v>
       </c>
       <c r="B75">
         <v>1</v>
@@ -80388,10 +80391,10 @@
         <v>0.66666666699999999</v>
       </c>
       <c r="E75">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F75">
-        <v>2.2999999999999998</v>
+        <v>1.25</v>
       </c>
       <c r="G75">
         <v>0</v>
@@ -80406,15 +80409,15 @@
         <v>10</v>
       </c>
       <c r="M75">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="B76">
-        <v>2.1</v>
+        <v>1</v>
       </c>
       <c r="C76">
         <v>1</v>
@@ -80423,10 +80426,10 @@
         <v>0.66666666699999999</v>
       </c>
       <c r="E76">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F76">
-        <v>2.5</v>
+        <v>0.7</v>
       </c>
       <c r="G76">
         <v>0</v>
@@ -80441,7 +80444,7 @@
         <v>10</v>
       </c>
       <c r="L76" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="M76">
         <v>1</v>
@@ -80449,7 +80452,7 @@
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>133</v>
+        <v>59</v>
       </c>
       <c r="B77">
         <v>1</v>
@@ -80461,10 +80464,10 @@
         <v>0.66666666699999999</v>
       </c>
       <c r="E77">
-        <v>3.3</v>
+        <v>3</v>
       </c>
       <c r="F77">
-        <v>2.2000000000000002</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="G77">
         <v>0</v>
@@ -80479,39 +80482,42 @@
         <v>10</v>
       </c>
       <c r="M77">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>318</v>
+        <v>60</v>
       </c>
       <c r="B78">
-        <v>22.5</v>
+        <v>2.1</v>
       </c>
       <c r="C78">
-        <v>1.25</v>
+        <v>1</v>
       </c>
       <c r="D78">
-        <v>0.83333333300000001</v>
+        <v>0.66666666699999999</v>
       </c>
       <c r="E78">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F78">
-        <v>0.01</v>
+        <v>2.5</v>
       </c>
       <c r="G78">
         <v>0</v>
       </c>
       <c r="H78" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I78" t="b">
         <v>1</v>
       </c>
       <c r="K78">
-        <v>0</v>
+        <v>10</v>
+      </c>
+      <c r="L78" t="s">
+        <v>67</v>
       </c>
       <c r="M78">
         <v>1</v>
@@ -80519,34 +80525,34 @@
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>320</v>
+        <v>133</v>
       </c>
       <c r="B79">
-        <v>42.75</v>
+        <v>1</v>
       </c>
       <c r="C79">
-        <v>1.25</v>
+        <v>1</v>
       </c>
       <c r="D79">
-        <v>0.83333333300000001</v>
+        <v>0.66666666699999999</v>
       </c>
       <c r="E79">
-        <v>2</v>
+        <v>3.3</v>
       </c>
       <c r="F79">
-        <v>2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="G79">
         <v>0</v>
       </c>
       <c r="H79" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I79" t="b">
         <v>1</v>
       </c>
       <c r="K79">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="M79">
         <v>1</v>
@@ -80554,22 +80560,22 @@
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>64</v>
+        <v>318</v>
       </c>
       <c r="B80">
-        <v>0.25</v>
+        <v>22.5</v>
       </c>
       <c r="C80">
-        <v>0.25</v>
+        <v>1.25</v>
       </c>
       <c r="D80">
-        <v>0.2</v>
+        <v>0.83333333300000001</v>
       </c>
       <c r="E80">
-        <v>2.2000000000000002</v>
+        <v>2</v>
       </c>
       <c r="F80">
-        <v>1.4</v>
+        <v>0.01</v>
       </c>
       <c r="G80">
         <v>0</v>
@@ -80584,27 +80590,27 @@
         <v>0</v>
       </c>
       <c r="M80">
-        <v>0.3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>202</v>
+        <v>320</v>
       </c>
       <c r="B81">
-        <v>0.25</v>
+        <v>42.75</v>
       </c>
       <c r="C81">
-        <v>0.32</v>
+        <v>1.25</v>
       </c>
       <c r="D81">
-        <v>0.2</v>
+        <v>0.83333333300000001</v>
       </c>
       <c r="E81">
-        <v>2.2000000000000002</v>
+        <v>2</v>
       </c>
       <c r="F81">
-        <v>1.4</v>
+        <v>2</v>
       </c>
       <c r="G81">
         <v>0</v>
@@ -80619,27 +80625,27 @@
         <v>0</v>
       </c>
       <c r="M81">
-        <v>0.3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>146</v>
+        <v>64</v>
       </c>
       <c r="B82">
-        <v>38.25</v>
+        <v>0.25</v>
       </c>
       <c r="C82">
-        <v>1.25</v>
+        <v>0.25</v>
       </c>
       <c r="D82">
-        <v>0.83333333300000001</v>
+        <v>0.2</v>
       </c>
       <c r="E82">
-        <v>2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="F82">
-        <v>2</v>
+        <v>1.4</v>
       </c>
       <c r="G82">
         <v>0</v>
@@ -80654,27 +80660,27 @@
         <v>0</v>
       </c>
       <c r="M82">
-        <v>5</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>1714</v>
+        <v>202</v>
       </c>
       <c r="B83">
-        <v>61.2</v>
+        <v>0.25</v>
       </c>
       <c r="C83">
-        <v>1.25</v>
+        <v>0.32</v>
       </c>
       <c r="D83">
-        <v>0.83333333300000001</v>
+        <v>0.2</v>
       </c>
       <c r="E83">
-        <v>2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="F83">
-        <v>2</v>
+        <v>1.4</v>
       </c>
       <c r="G83">
         <v>0</v>
@@ -80689,15 +80695,15 @@
         <v>0</v>
       </c>
       <c r="M83">
-        <v>5</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B84">
-        <v>51.75</v>
+        <v>38.25</v>
       </c>
       <c r="C84">
         <v>1.25</v>
@@ -80709,7 +80715,7 @@
         <v>2</v>
       </c>
       <c r="F84">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G84">
         <v>0</v>
@@ -80729,10 +80735,10 @@
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>517</v>
+        <v>1714</v>
       </c>
       <c r="B85">
-        <v>51.75</v>
+        <v>61.2</v>
       </c>
       <c r="C85">
         <v>1.25</v>
@@ -80764,10 +80770,10 @@
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B86">
-        <v>47.25</v>
+        <v>51.75</v>
       </c>
       <c r="C86">
         <v>1.25</v>
@@ -80779,7 +80785,7 @@
         <v>2</v>
       </c>
       <c r="F86">
-        <v>0.01</v>
+        <v>5</v>
       </c>
       <c r="G86">
         <v>0</v>
@@ -80794,15 +80800,15 @@
         <v>0</v>
       </c>
       <c r="M86">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>332</v>
+        <v>517</v>
       </c>
       <c r="B87">
-        <v>36</v>
+        <v>51.75</v>
       </c>
       <c r="C87">
         <v>1.25</v>
@@ -80834,10 +80840,10 @@
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>518</v>
+        <v>148</v>
       </c>
       <c r="B88">
-        <v>42.75</v>
+        <v>47.25</v>
       </c>
       <c r="C88">
         <v>1.25</v>
@@ -80849,7 +80855,7 @@
         <v>2</v>
       </c>
       <c r="F88">
-        <v>2</v>
+        <v>0.01</v>
       </c>
       <c r="G88">
         <v>0</v>
@@ -80864,15 +80870,15 @@
         <v>0</v>
       </c>
       <c r="M88">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B89">
-        <v>18.899999999999999</v>
+        <v>36</v>
       </c>
       <c r="C89">
         <v>1.25</v>
@@ -80899,27 +80905,27 @@
         <v>0</v>
       </c>
       <c r="M89">
-        <v>0.1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>524</v>
+        <v>518</v>
       </c>
       <c r="B90">
-        <v>0.7</v>
+        <v>42.75</v>
       </c>
       <c r="C90">
-        <v>0.45</v>
+        <v>1.25</v>
       </c>
       <c r="D90">
-        <v>0.2</v>
+        <v>0.83333333300000001</v>
       </c>
       <c r="E90">
         <v>2</v>
       </c>
       <c r="F90">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G90">
         <v>0</v>
@@ -80934,27 +80940,27 @@
         <v>0</v>
       </c>
       <c r="M90">
-        <v>0.3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>153</v>
+        <v>333</v>
       </c>
       <c r="B91">
-        <v>1.05</v>
+        <v>18.899999999999999</v>
       </c>
       <c r="C91">
-        <v>0.3</v>
+        <v>1.25</v>
       </c>
       <c r="D91">
-        <v>0.2</v>
+        <v>0.83333333300000001</v>
       </c>
       <c r="E91">
         <v>2</v>
       </c>
       <c r="F91">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G91">
         <v>0</v>
@@ -80969,18 +80975,18 @@
         <v>0</v>
       </c>
       <c r="M91">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="B92">
-        <v>0.84</v>
+        <v>0.7</v>
       </c>
       <c r="C92">
-        <v>0.3</v>
+        <v>0.45</v>
       </c>
       <c r="D92">
         <v>0.2</v>
@@ -81009,22 +81015,22 @@
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="B93">
-        <v>54</v>
+        <v>1.05</v>
       </c>
       <c r="C93">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="D93">
-        <v>0.83333333300000001</v>
+        <v>0.2</v>
       </c>
       <c r="E93">
         <v>2</v>
       </c>
       <c r="F93">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G93">
         <v>0</v>
@@ -81039,27 +81045,27 @@
         <v>0</v>
       </c>
       <c r="M93">
-        <v>5</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>152</v>
+        <v>523</v>
       </c>
       <c r="B94">
-        <v>49.5</v>
+        <v>0.84</v>
       </c>
       <c r="C94">
-        <v>1.25</v>
+        <v>0.3</v>
       </c>
       <c r="D94">
-        <v>0.83333333300000001</v>
+        <v>0.2</v>
       </c>
       <c r="E94">
         <v>2</v>
       </c>
       <c r="F94">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G94">
         <v>0</v>
@@ -81074,18 +81080,18 @@
         <v>0</v>
       </c>
       <c r="M94">
-        <v>5</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="95" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="B95">
-        <v>43.2</v>
+        <v>54</v>
       </c>
       <c r="C95">
-        <v>1.25</v>
+        <v>0.5</v>
       </c>
       <c r="D95">
         <v>0.83333333300000001</v>
@@ -81094,7 +81100,7 @@
         <v>2</v>
       </c>
       <c r="F95">
-        <v>2.75</v>
+        <v>2</v>
       </c>
       <c r="G95">
         <v>0</v>
@@ -81114,10 +81120,10 @@
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B96">
-        <v>47.25</v>
+        <v>49.5</v>
       </c>
       <c r="C96">
         <v>1.25</v>
@@ -81129,7 +81135,7 @@
         <v>2</v>
       </c>
       <c r="F96">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="G96">
         <v>0</v>
@@ -81149,10 +81155,10 @@
     </row>
     <row r="97" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>1813</v>
+        <v>158</v>
       </c>
       <c r="B97">
-        <v>33.75</v>
+        <v>43.2</v>
       </c>
       <c r="C97">
         <v>1.25</v>
@@ -81164,7 +81170,7 @@
         <v>2</v>
       </c>
       <c r="F97">
-        <v>2.5</v>
+        <v>2.75</v>
       </c>
       <c r="G97">
         <v>0</v>
@@ -81184,10 +81190,10 @@
     </row>
     <row r="98" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="B98">
-        <v>58.5</v>
+        <v>47.25</v>
       </c>
       <c r="C98">
         <v>1.25</v>
@@ -81199,7 +81205,7 @@
         <v>2</v>
       </c>
       <c r="F98">
-        <v>3.75</v>
+        <v>2.5</v>
       </c>
       <c r="G98">
         <v>0</v>
@@ -81219,10 +81225,10 @@
     </row>
     <row r="99" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>160</v>
+        <v>1813</v>
       </c>
       <c r="B99">
-        <v>23.265000000000001</v>
+        <v>33.75</v>
       </c>
       <c r="C99">
         <v>1.25</v>
@@ -81234,7 +81240,7 @@
         <v>2</v>
       </c>
       <c r="F99">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="G99">
         <v>0</v>
@@ -81249,15 +81255,15 @@
         <v>0</v>
       </c>
       <c r="M99">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="100" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B100">
-        <v>36</v>
+        <v>58.5</v>
       </c>
       <c r="C100">
         <v>1.25</v>
@@ -81269,7 +81275,7 @@
         <v>2</v>
       </c>
       <c r="F100">
-        <v>2</v>
+        <v>3.75</v>
       </c>
       <c r="G100">
         <v>0</v>
@@ -81284,15 +81290,15 @@
         <v>0</v>
       </c>
       <c r="M100">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="101" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>1715</v>
+        <v>160</v>
       </c>
       <c r="B101">
-        <v>38.25</v>
+        <v>23.265000000000001</v>
       </c>
       <c r="C101">
         <v>1.25</v>
@@ -81319,15 +81325,15 @@
         <v>0</v>
       </c>
       <c r="M101">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="102" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>925</v>
+        <v>161</v>
       </c>
       <c r="B102">
-        <v>52.875</v>
+        <v>36</v>
       </c>
       <c r="C102">
         <v>1.25</v>
@@ -81354,15 +81360,15 @@
         <v>0</v>
       </c>
       <c r="M102">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="103" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>1716</v>
+        <v>1715</v>
       </c>
       <c r="B103">
-        <v>54</v>
+        <v>38.25</v>
       </c>
       <c r="C103">
         <v>1.25</v>
@@ -81389,15 +81395,15 @@
         <v>0</v>
       </c>
       <c r="M103">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="104" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>720</v>
+        <v>925</v>
       </c>
       <c r="B104">
-        <v>49.5</v>
+        <v>52.875</v>
       </c>
       <c r="C104">
         <v>1.25</v>
@@ -81409,7 +81415,7 @@
         <v>2</v>
       </c>
       <c r="F104">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G104">
         <v>0</v>
@@ -81429,7 +81435,7 @@
     </row>
     <row r="105" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>924</v>
+        <v>1716</v>
       </c>
       <c r="B105">
         <v>54</v>
@@ -81464,10 +81470,10 @@
     </row>
     <row r="106" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>923</v>
+        <v>720</v>
       </c>
       <c r="B106">
-        <v>87.75</v>
+        <v>49.5</v>
       </c>
       <c r="C106">
         <v>1.25</v>
@@ -81479,7 +81485,7 @@
         <v>2</v>
       </c>
       <c r="F106">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G106">
         <v>0</v>
@@ -81499,10 +81505,10 @@
     </row>
     <row r="107" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>1814</v>
+        <v>924</v>
       </c>
       <c r="B107">
-        <v>78.75</v>
+        <v>54</v>
       </c>
       <c r="C107">
         <v>1.25</v>
@@ -81534,10 +81540,10 @@
     </row>
     <row r="108" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>939</v>
+        <v>923</v>
       </c>
       <c r="B108">
-        <v>47.924999999999997</v>
+        <v>87.75</v>
       </c>
       <c r="C108">
         <v>1.25</v>
@@ -81566,16 +81572,13 @@
       <c r="M108">
         <v>1</v>
       </c>
-      <c r="N108">
-        <v>0.01</v>
-      </c>
     </row>
     <row r="109" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>926</v>
+        <v>1814</v>
       </c>
       <c r="B109">
-        <v>36.825000000000003</v>
+        <v>78.75</v>
       </c>
       <c r="C109">
         <v>1.25</v>
@@ -81604,16 +81607,13 @@
       <c r="M109">
         <v>1</v>
       </c>
-      <c r="N109">
-        <v>0.01</v>
-      </c>
     </row>
     <row r="110" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>1027</v>
+        <v>939</v>
       </c>
       <c r="B110">
-        <v>21.824999999999999</v>
+        <v>47.924999999999997</v>
       </c>
       <c r="C110">
         <v>1.25</v>
@@ -81642,13 +81642,16 @@
       <c r="M110">
         <v>1</v>
       </c>
+      <c r="N110">
+        <v>0.01</v>
+      </c>
     </row>
     <row r="111" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>1031</v>
+        <v>926</v>
       </c>
       <c r="B111">
-        <v>0.5</v>
+        <v>36.825000000000003</v>
       </c>
       <c r="C111">
         <v>1.25</v>
@@ -81677,13 +81680,16 @@
       <c r="M111">
         <v>1</v>
       </c>
+      <c r="N111">
+        <v>0.01</v>
+      </c>
     </row>
     <row r="112" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>1032</v>
+        <v>1027</v>
       </c>
       <c r="B112">
-        <v>47.25</v>
+        <v>21.824999999999999</v>
       </c>
       <c r="C112">
         <v>1.25</v>
@@ -81715,10 +81721,10 @@
     </row>
     <row r="113" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>1028</v>
+        <v>1031</v>
       </c>
       <c r="B113">
-        <v>69.75</v>
+        <v>0.5</v>
       </c>
       <c r="C113">
         <v>1.25</v>
@@ -81730,7 +81736,7 @@
         <v>2</v>
       </c>
       <c r="F113">
-        <v>4.5</v>
+        <v>2</v>
       </c>
       <c r="G113">
         <v>0</v>
@@ -81750,10 +81756,10 @@
     </row>
     <row r="114" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>1029</v>
+        <v>1032</v>
       </c>
       <c r="B114">
-        <v>72</v>
+        <v>47.25</v>
       </c>
       <c r="C114">
         <v>1.25</v>
@@ -81765,7 +81771,7 @@
         <v>2</v>
       </c>
       <c r="F114">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G114">
         <v>0</v>
@@ -81778,9 +81784,6 @@
       </c>
       <c r="K114">
         <v>0</v>
-      </c>
-      <c r="L114" t="s">
-        <v>1249</v>
       </c>
       <c r="M114">
         <v>1</v>
@@ -81788,10 +81791,10 @@
     </row>
     <row r="115" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>1717</v>
+        <v>1028</v>
       </c>
       <c r="B115">
-        <v>74.25</v>
+        <v>69.75</v>
       </c>
       <c r="C115">
         <v>1.25</v>
@@ -81803,7 +81806,7 @@
         <v>2</v>
       </c>
       <c r="F115">
-        <v>7</v>
+        <v>4.5</v>
       </c>
       <c r="G115">
         <v>0</v>
@@ -81816,9 +81819,6 @@
       </c>
       <c r="K115">
         <v>0</v>
-      </c>
-      <c r="L115" t="s">
-        <v>1249</v>
       </c>
       <c r="M115">
         <v>1</v>
@@ -81826,10 +81826,10 @@
     </row>
     <row r="116" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>1257</v>
+        <v>1029</v>
       </c>
       <c r="B116">
-        <v>42.75</v>
+        <v>72</v>
       </c>
       <c r="C116">
         <v>1.25</v>
@@ -81841,7 +81841,7 @@
         <v>2</v>
       </c>
       <c r="F116">
-        <v>3.5</v>
+        <v>7</v>
       </c>
       <c r="G116">
         <v>0</v>
@@ -81854,6 +81854,9 @@
       </c>
       <c r="K116">
         <v>0</v>
+      </c>
+      <c r="L116" t="s">
+        <v>1249</v>
       </c>
       <c r="M116">
         <v>1</v>
@@ -81861,10 +81864,10 @@
     </row>
     <row r="117" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>1261</v>
+        <v>1717</v>
       </c>
       <c r="B117">
-        <v>13.5</v>
+        <v>74.25</v>
       </c>
       <c r="C117">
         <v>1.25</v>
@@ -81876,7 +81879,7 @@
         <v>2</v>
       </c>
       <c r="F117">
-        <v>1.3</v>
+        <v>7</v>
       </c>
       <c r="G117">
         <v>0</v>
@@ -81889,6 +81892,9 @@
       </c>
       <c r="K117">
         <v>0</v>
+      </c>
+      <c r="L117" t="s">
+        <v>1249</v>
       </c>
       <c r="M117">
         <v>1</v>
@@ -81896,10 +81902,10 @@
     </row>
     <row r="118" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>1262</v>
+        <v>1257</v>
       </c>
       <c r="B118">
-        <v>20.25</v>
+        <v>42.75</v>
       </c>
       <c r="C118">
         <v>1.25</v>
@@ -81911,7 +81917,7 @@
         <v>2</v>
       </c>
       <c r="F118">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="G118">
         <v>0</v>
@@ -81931,10 +81937,10 @@
     </row>
     <row r="119" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>1263</v>
+        <v>1261</v>
       </c>
       <c r="B119">
-        <v>15.75</v>
+        <v>13.5</v>
       </c>
       <c r="C119">
         <v>1.25</v>
@@ -81946,7 +81952,7 @@
         <v>2</v>
       </c>
       <c r="F119">
-        <v>4.5</v>
+        <v>1.3</v>
       </c>
       <c r="G119">
         <v>0</v>
@@ -81966,10 +81972,10 @@
     </row>
     <row r="120" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>1264</v>
+        <v>1262</v>
       </c>
       <c r="B120">
-        <v>56.25</v>
+        <v>20.25</v>
       </c>
       <c r="C120">
         <v>1.25</v>
@@ -81981,7 +81987,7 @@
         <v>2</v>
       </c>
       <c r="F120">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="G120">
         <v>0</v>
@@ -82001,10 +82007,10 @@
     </row>
     <row r="121" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>1258</v>
+        <v>1263</v>
       </c>
       <c r="B121">
-        <v>1</v>
+        <v>15.75</v>
       </c>
       <c r="C121">
         <v>1.25</v>
@@ -82016,7 +82022,7 @@
         <v>2</v>
       </c>
       <c r="F121">
-        <v>1.25</v>
+        <v>4.5</v>
       </c>
       <c r="G121">
         <v>0</v>
@@ -82032,17 +82038,14 @@
       </c>
       <c r="M121">
         <v>1</v>
-      </c>
-      <c r="N121">
-        <v>0.1</v>
       </c>
     </row>
     <row r="122" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
       <c r="B122">
-        <v>3.5</v>
+        <v>56.25</v>
       </c>
       <c r="C122">
         <v>1.25</v>
@@ -82054,7 +82057,7 @@
         <v>2</v>
       </c>
       <c r="F122">
-        <v>0.01</v>
+        <v>2.5</v>
       </c>
       <c r="G122">
         <v>0</v>
@@ -82069,18 +82072,15 @@
         <v>0</v>
       </c>
       <c r="M122">
-        <v>0.1</v>
-      </c>
-      <c r="N122">
-        <v>0.01</v>
+        <v>1</v>
       </c>
     </row>
     <row r="123" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>329</v>
+        <v>1258</v>
       </c>
       <c r="B123">
-        <v>54</v>
+        <v>1</v>
       </c>
       <c r="C123">
         <v>1.25</v>
@@ -82092,7 +82092,7 @@
         <v>2</v>
       </c>
       <c r="F123">
-        <v>5</v>
+        <v>1.25</v>
       </c>
       <c r="G123">
         <v>0</v>
@@ -82106,19 +82106,19 @@
       <c r="K123">
         <v>0</v>
       </c>
-      <c r="L123" t="s">
-        <v>1252</v>
-      </c>
       <c r="M123">
         <v>1</v>
+      </c>
+      <c r="N123">
+        <v>0.1</v>
       </c>
     </row>
     <row r="124" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>1718</v>
+        <v>1265</v>
       </c>
       <c r="B124">
-        <v>76.5</v>
+        <v>3.5</v>
       </c>
       <c r="C124">
         <v>1.25</v>
@@ -82130,7 +82130,7 @@
         <v>2</v>
       </c>
       <c r="F124">
-        <v>3</v>
+        <v>0.01</v>
       </c>
       <c r="G124">
         <v>0</v>
@@ -82145,15 +82145,18 @@
         <v>0</v>
       </c>
       <c r="M124">
-        <v>1</v>
+        <v>0.1</v>
+      </c>
+      <c r="N124">
+        <v>0.01</v>
       </c>
     </row>
     <row r="125" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>1037</v>
+        <v>329</v>
       </c>
       <c r="B125">
-        <v>40.5</v>
+        <v>54</v>
       </c>
       <c r="C125">
         <v>1.25</v>
@@ -82165,7 +82168,7 @@
         <v>2</v>
       </c>
       <c r="F125">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G125">
         <v>0</v>
@@ -82178,6 +82181,9 @@
       </c>
       <c r="K125">
         <v>0</v>
+      </c>
+      <c r="L125" t="s">
+        <v>1252</v>
       </c>
       <c r="M125">
         <v>1</v>
@@ -82185,28 +82191,28 @@
     </row>
     <row r="126" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>1034</v>
+        <v>1718</v>
       </c>
       <c r="B126">
-        <v>15</v>
+        <v>76.5</v>
       </c>
       <c r="C126">
-        <v>1</v>
+        <v>1.25</v>
       </c>
       <c r="D126">
-        <v>0.66666666699999999</v>
+        <v>0.83333333300000001</v>
       </c>
       <c r="E126">
         <v>2</v>
       </c>
       <c r="F126">
-        <v>0.01</v>
+        <v>3</v>
       </c>
       <c r="G126">
         <v>0</v>
       </c>
       <c r="H126" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I126" t="b">
         <v>1</v>
@@ -82220,10 +82226,10 @@
     </row>
     <row r="127" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>1039</v>
+        <v>1037</v>
       </c>
       <c r="B127">
-        <v>47.25</v>
+        <v>40.5</v>
       </c>
       <c r="C127">
         <v>1.25</v>
@@ -82235,7 +82241,7 @@
         <v>2</v>
       </c>
       <c r="F127">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G127">
         <v>0</v>
@@ -82248,9 +82254,6 @@
       </c>
       <c r="K127">
         <v>0</v>
-      </c>
-      <c r="L127" t="s">
-        <v>1252</v>
       </c>
       <c r="M127">
         <v>1</v>
@@ -82258,28 +82261,28 @@
     </row>
     <row r="128" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>1815</v>
+        <v>1034</v>
       </c>
       <c r="B128">
-        <v>54</v>
+        <v>15</v>
       </c>
       <c r="C128">
-        <v>1.25</v>
+        <v>1</v>
       </c>
       <c r="D128">
-        <v>0.83333333300000001</v>
+        <v>0.66666666699999999</v>
       </c>
       <c r="E128">
         <v>2</v>
       </c>
       <c r="F128">
-        <v>2</v>
+        <v>0.01</v>
       </c>
       <c r="G128">
         <v>0</v>
       </c>
       <c r="H128" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I128" t="b">
         <v>1</v>
@@ -82293,10 +82296,10 @@
     </row>
     <row r="129" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>2198</v>
+        <v>1039</v>
       </c>
       <c r="B129">
-        <v>58.5</v>
+        <v>47.25</v>
       </c>
       <c r="C129">
         <v>1.25</v>
@@ -82308,7 +82311,7 @@
         <v>2</v>
       </c>
       <c r="F129">
-        <v>0.01</v>
+        <v>2</v>
       </c>
       <c r="G129">
         <v>0</v>
@@ -82322,19 +82325,19 @@
       <c r="K129">
         <v>0</v>
       </c>
+      <c r="L129" t="s">
+        <v>1252</v>
+      </c>
       <c r="M129">
-        <v>0.3</v>
-      </c>
-      <c r="N129">
-        <v>0.01</v>
+        <v>1</v>
       </c>
     </row>
     <row r="130" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>2199</v>
+        <v>1815</v>
       </c>
       <c r="B130">
-        <v>58.5</v>
+        <v>54</v>
       </c>
       <c r="C130">
         <v>1.25</v>
@@ -82346,7 +82349,7 @@
         <v>2</v>
       </c>
       <c r="F130">
-        <v>0.01</v>
+        <v>2</v>
       </c>
       <c r="G130">
         <v>0</v>
@@ -82361,30 +82364,27 @@
         <v>0</v>
       </c>
       <c r="M130">
-        <v>0.3</v>
-      </c>
-      <c r="N130">
-        <v>0.01</v>
+        <v>1</v>
       </c>
     </row>
     <row r="131" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>2203</v>
+        <v>2198</v>
       </c>
       <c r="B131">
-        <v>0.7</v>
+        <v>58.5</v>
       </c>
       <c r="C131">
-        <v>0.6</v>
+        <v>1.25</v>
       </c>
       <c r="D131">
-        <v>0.4</v>
+        <v>0.83333333300000001</v>
       </c>
       <c r="E131">
         <v>2</v>
       </c>
       <c r="F131">
-        <v>2.5</v>
+        <v>0.01</v>
       </c>
       <c r="G131">
         <v>0</v>
@@ -82399,15 +82399,18 @@
         <v>0</v>
       </c>
       <c r="M131">
-        <v>1</v>
+        <v>0.3</v>
+      </c>
+      <c r="N131">
+        <v>0.01</v>
       </c>
     </row>
     <row r="132" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>2200</v>
+        <v>2199</v>
       </c>
       <c r="B132">
-        <v>45</v>
+        <v>58.5</v>
       </c>
       <c r="C132">
         <v>1.25</v>
@@ -82419,7 +82422,7 @@
         <v>2</v>
       </c>
       <c r="F132">
-        <v>1.5</v>
+        <v>0.01</v>
       </c>
       <c r="G132">
         <v>0</v>
@@ -82434,27 +82437,30 @@
         <v>0</v>
       </c>
       <c r="M132">
-        <v>0.5</v>
+        <v>0.3</v>
+      </c>
+      <c r="N132">
+        <v>0.01</v>
       </c>
     </row>
     <row r="133" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>2431</v>
+        <v>2203</v>
       </c>
       <c r="B133">
-        <v>45</v>
+        <v>0.7</v>
       </c>
       <c r="C133">
-        <v>1.25</v>
+        <v>0.6</v>
       </c>
       <c r="D133">
-        <v>0.83333333300000001</v>
+        <v>0.4</v>
       </c>
       <c r="E133">
         <v>2</v>
       </c>
       <c r="F133">
-        <v>3.5</v>
+        <v>2.5</v>
       </c>
       <c r="G133">
         <v>0</v>
@@ -82474,7 +82480,7 @@
     </row>
     <row r="134" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>1266</v>
+        <v>2200</v>
       </c>
       <c r="B134">
         <v>45</v>
@@ -82489,7 +82495,7 @@
         <v>2</v>
       </c>
       <c r="F134">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="G134">
         <v>0</v>
@@ -82504,12 +82510,12 @@
         <v>0</v>
       </c>
       <c r="M134">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="135" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>327</v>
+        <v>2431</v>
       </c>
       <c r="B135">
         <v>45</v>
@@ -82524,7 +82530,7 @@
         <v>2</v>
       </c>
       <c r="F135">
-        <v>2</v>
+        <v>3.5</v>
       </c>
       <c r="G135">
         <v>0</v>
@@ -82544,7 +82550,7 @@
     </row>
     <row r="136" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>328</v>
+        <v>1266</v>
       </c>
       <c r="B136">
         <v>45</v>
@@ -82574,21 +82580,21 @@
         <v>0</v>
       </c>
       <c r="M136">
-        <v>1</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="137" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>1017</v>
+        <v>327</v>
       </c>
       <c r="B137">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="C137">
-        <v>1</v>
+        <v>1.25</v>
       </c>
       <c r="D137">
-        <v>1</v>
+        <v>0.83333333300000001</v>
       </c>
       <c r="E137">
         <v>2</v>
@@ -82600,13 +82606,13 @@
         <v>0</v>
       </c>
       <c r="H137" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I137" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K137">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M137">
         <v>1</v>
@@ -82614,16 +82620,16 @@
     </row>
     <row r="138" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>1020</v>
+        <v>328</v>
       </c>
       <c r="B138">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="C138">
-        <v>1</v>
+        <v>1.25</v>
       </c>
       <c r="D138">
-        <v>1</v>
+        <v>0.83333333300000001</v>
       </c>
       <c r="E138">
         <v>2</v>
@@ -82635,13 +82641,13 @@
         <v>0</v>
       </c>
       <c r="H138" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I138" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K138">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M138">
         <v>1</v>
@@ -82649,10 +82655,10 @@
     </row>
     <row r="139" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>1015</v>
+        <v>1017</v>
       </c>
       <c r="B139">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C139">
         <v>1</v>
@@ -82664,7 +82670,7 @@
         <v>2</v>
       </c>
       <c r="F139">
-        <v>3.8</v>
+        <v>2</v>
       </c>
       <c r="G139">
         <v>0</v>
@@ -82684,13 +82690,13 @@
     </row>
     <row r="140" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>1016</v>
+        <v>1020</v>
       </c>
       <c r="B140">
-        <v>1.25</v>
+        <v>1</v>
       </c>
       <c r="C140">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="D140">
         <v>1</v>
@@ -82699,7 +82705,7 @@
         <v>2</v>
       </c>
       <c r="F140">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="G140">
         <v>0</v>
@@ -82719,13 +82725,13 @@
     </row>
     <row r="141" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>1018</v>
+        <v>1015</v>
       </c>
       <c r="B141">
-        <v>4.2</v>
+        <v>0.5</v>
       </c>
       <c r="C141">
-        <v>1.3</v>
+        <v>1</v>
       </c>
       <c r="D141">
         <v>1</v>
@@ -82734,7 +82740,7 @@
         <v>2</v>
       </c>
       <c r="F141">
-        <v>0.6</v>
+        <v>3.8</v>
       </c>
       <c r="G141">
         <v>0</v>
@@ -82754,13 +82760,13 @@
     </row>
     <row r="142" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>1019</v>
+        <v>1016</v>
       </c>
       <c r="B142">
-        <v>6</v>
+        <v>1.25</v>
       </c>
       <c r="C142">
-        <v>1.75</v>
+        <v>0.7</v>
       </c>
       <c r="D142">
         <v>1</v>
@@ -82769,7 +82775,7 @@
         <v>2</v>
       </c>
       <c r="F142">
-        <v>3.2</v>
+        <v>2.5</v>
       </c>
       <c r="G142">
         <v>0</v>
@@ -82789,13 +82795,13 @@
     </row>
     <row r="143" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>1021</v>
+        <v>1018</v>
       </c>
       <c r="B143">
-        <v>0.24</v>
+        <v>4.2</v>
       </c>
       <c r="C143">
-        <v>2</v>
+        <v>1.3</v>
       </c>
       <c r="D143">
         <v>1</v>
@@ -82804,7 +82810,7 @@
         <v>2</v>
       </c>
       <c r="F143">
-        <v>4.2</v>
+        <v>0.6</v>
       </c>
       <c r="G143">
         <v>0</v>
@@ -82824,36 +82830,106 @@
     </row>
     <row r="144" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
+        <v>1019</v>
+      </c>
+      <c r="B144">
+        <v>6</v>
+      </c>
+      <c r="C144">
+        <v>1.75</v>
+      </c>
+      <c r="D144">
+        <v>1</v>
+      </c>
+      <c r="E144">
+        <v>2</v>
+      </c>
+      <c r="F144">
+        <v>3.2</v>
+      </c>
+      <c r="G144">
+        <v>0</v>
+      </c>
+      <c r="H144" t="b">
+        <v>0</v>
+      </c>
+      <c r="I144" t="b">
+        <v>0</v>
+      </c>
+      <c r="K144">
+        <v>2</v>
+      </c>
+      <c r="M144">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A145" t="s">
+        <v>1021</v>
+      </c>
+      <c r="B145">
+        <v>0.24</v>
+      </c>
+      <c r="C145">
+        <v>2</v>
+      </c>
+      <c r="D145">
+        <v>1</v>
+      </c>
+      <c r="E145">
+        <v>2</v>
+      </c>
+      <c r="F145">
+        <v>4.2</v>
+      </c>
+      <c r="G145">
+        <v>0</v>
+      </c>
+      <c r="H145" t="b">
+        <v>0</v>
+      </c>
+      <c r="I145" t="b">
+        <v>0</v>
+      </c>
+      <c r="K145">
+        <v>2</v>
+      </c>
+      <c r="M145">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A146" t="s">
         <v>1024</v>
       </c>
-      <c r="B144">
+      <c r="B146">
         <v>0.375</v>
       </c>
-      <c r="C144">
+      <c r="C146">
         <v>0.45500000000000002</v>
       </c>
-      <c r="D144">
-        <v>1</v>
-      </c>
-      <c r="E144">
+      <c r="D146">
+        <v>1</v>
+      </c>
+      <c r="E146">
         <v>0.2</v>
       </c>
-      <c r="F144">
+      <c r="F146">
         <v>0.01</v>
       </c>
-      <c r="G144">
-        <v>0</v>
-      </c>
-      <c r="H144" t="b">
-        <v>0</v>
-      </c>
-      <c r="I144" t="b">
-        <v>0</v>
-      </c>
-      <c r="K144">
-        <v>0</v>
-      </c>
-      <c r="M144">
+      <c r="G146">
+        <v>0</v>
+      </c>
+      <c r="H146" t="b">
+        <v>0</v>
+      </c>
+      <c r="I146" t="b">
+        <v>0</v>
+      </c>
+      <c r="K146">
+        <v>0</v>
+      </c>
+      <c r="M146">
         <v>0.1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
챕터테이블 standardPowerLevel 컬럼 추가
</commit_message>
<xml_diff>
--- a/Excel/Stage.xlsx
+++ b/Excel/Stage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectNoname\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB89FE34-B280-4726-92AE-7AF202451FDF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35A76424-E5B3-4393-B6F9-FD5B738EA051}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{566BA174-F383-48D7-A97F-7F70BBC36EC1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{566BA174-F383-48D7-A97F-7F70BBC36EC1}"/>
   </bookViews>
   <sheets>
     <sheet name="ChapterTable" sheetId="5" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6918" uniqueCount="2935">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6924" uniqueCount="2940">
   <si>
     <t>chapter|Int</t>
   </si>
@@ -8842,6 +8842,22 @@
   </si>
   <si>
     <t>Actor3114, Actor2235</t>
+  </si>
+  <si>
+    <t>Chapter15Name</t>
+  </si>
+  <si>
+    <t>Chapter15Desc</t>
+  </si>
+  <si>
+    <t>c8014</t>
+  </si>
+  <si>
+    <t>c9014</t>
+  </si>
+  <si>
+    <t>standardPowerLevel|Float</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -9211,19 +9227,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBA5F51C-E5AC-4807-B5DA-B04AF572E74F}">
-  <dimension ref="A1:M16"/>
+  <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="6" width="14.5" customWidth="1"/>
-    <col min="7" max="7" width="17.75" customWidth="1"/>
+    <col min="7" max="7" width="14.5" customWidth="1"/>
+    <col min="8" max="8" width="17.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -9240,31 +9256,34 @@
         <v>321</v>
       </c>
       <c r="F1" t="s">
+        <v>2939</v>
+      </c>
+      <c r="G1" t="s">
         <v>96</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>80</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>2438</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>2439</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>1803</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>1019</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>2090</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>2091</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -9277,17 +9296,20 @@
       <c r="E2">
         <v>1</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
         <v>1008</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>1009</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>1020</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -9300,17 +9322,20 @@
       <c r="E3">
         <v>2</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
         <v>97</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>81</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>1020</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -9323,17 +9348,20 @@
       <c r="E4">
         <v>3</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4">
+        <v>1.5</v>
+      </c>
+      <c r="G4" t="s">
         <v>98</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>82</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>1020</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -9346,17 +9374,20 @@
       <c r="E5">
         <v>4</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5">
+        <v>2</v>
+      </c>
+      <c r="G5" t="s">
         <v>99</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>83</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>1020</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -9372,26 +9403,29 @@
       <c r="E6">
         <v>5</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="G6" t="s">
         <v>100</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>84</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>2440</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>2441</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>100</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>1020</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -9407,26 +9441,29 @@
       <c r="E7">
         <v>5</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7">
+        <v>3</v>
+      </c>
+      <c r="G7" t="s">
         <v>101</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>85</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>2442</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>2443</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>240</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>1020</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -9442,26 +9479,29 @@
       <c r="E8">
         <v>6</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8">
+        <v>3.5</v>
+      </c>
+      <c r="G8" t="s">
         <v>102</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>86</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>2444</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>2445</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>520</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>1020</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -9477,26 +9517,29 @@
       <c r="E9">
         <v>7</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9">
+        <v>4.5</v>
+      </c>
+      <c r="G9" t="s">
         <v>103</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>87</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>2446</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>2447</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>860</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>1020</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -9512,26 +9555,29 @@
       <c r="E10">
         <v>8</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10">
+        <v>5</v>
+      </c>
+      <c r="G10" t="s">
         <v>104</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>88</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>2448</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>2449</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <v>430</v>
       </c>
-      <c r="K10" t="s">
+      <c r="L10" t="s">
         <v>1020</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -9547,26 +9593,29 @@
       <c r="E11">
         <v>9</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11">
+        <v>5.5</v>
+      </c>
+      <c r="G11" t="s">
         <v>105</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>89</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
         <v>2450</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
         <v>2451</v>
       </c>
-      <c r="J11">
+      <c r="K11">
         <v>460</v>
       </c>
-      <c r="K11" t="s">
+      <c r="L11" t="s">
         <v>1020</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -9582,26 +9631,29 @@
       <c r="E12">
         <v>9</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12">
+        <v>6</v>
+      </c>
+      <c r="G12" t="s">
         <v>106</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>90</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
         <v>2452</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
         <v>2453</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <v>540</v>
       </c>
-      <c r="K12" t="s">
+      <c r="L12" t="s">
         <v>1020</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
@@ -9617,26 +9669,29 @@
       <c r="E13">
         <v>10</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13">
+        <v>6.5</v>
+      </c>
+      <c r="G13" t="s">
         <v>107</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>91</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I13" t="s">
         <v>2454</v>
       </c>
-      <c r="I13" t="s">
+      <c r="J13" t="s">
         <v>2455</v>
       </c>
-      <c r="J13">
+      <c r="K13">
         <v>680</v>
       </c>
-      <c r="K13" t="s">
+      <c r="L13" t="s">
         <v>1020</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
@@ -9652,26 +9707,29 @@
       <c r="E14">
         <v>10</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14">
+        <v>7</v>
+      </c>
+      <c r="G14" t="s">
         <v>108</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
         <v>92</v>
       </c>
-      <c r="H14" t="s">
+      <c r="I14" t="s">
         <v>2456</v>
       </c>
-      <c r="I14" t="s">
+      <c r="J14" t="s">
         <v>2457</v>
       </c>
-      <c r="J14">
+      <c r="K14">
         <v>820</v>
       </c>
-      <c r="K14" t="s">
+      <c r="L14" t="s">
         <v>1020</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
@@ -9687,26 +9745,29 @@
       <c r="E15">
         <v>11</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15">
+        <v>8</v>
+      </c>
+      <c r="G15" t="s">
         <v>109</v>
       </c>
-      <c r="G15" t="s">
+      <c r="H15" t="s">
         <v>93</v>
       </c>
-      <c r="H15" t="s">
+      <c r="I15" t="s">
         <v>2458</v>
       </c>
-      <c r="I15" t="s">
+      <c r="J15" t="s">
         <v>2459</v>
       </c>
-      <c r="J15">
+      <c r="K15">
         <v>900</v>
       </c>
-      <c r="K15" t="s">
+      <c r="L15" t="s">
         <v>1020</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
@@ -9722,23 +9783,70 @@
       <c r="E16">
         <v>12</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16">
+        <v>9</v>
+      </c>
+      <c r="G16" t="s">
         <v>110</v>
       </c>
-      <c r="G16" t="s">
+      <c r="H16" t="s">
         <v>94</v>
       </c>
-      <c r="H16" t="s">
+      <c r="I16" t="s">
         <v>2460</v>
       </c>
-      <c r="I16" t="s">
+      <c r="J16" t="s">
         <v>2461</v>
       </c>
-      <c r="J16">
+      <c r="K16">
         <v>930</v>
       </c>
-      <c r="K16" t="s">
+      <c r="L16" t="s">
         <v>1020</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>50</v>
+      </c>
+      <c r="C17">
+        <v>50</v>
+      </c>
+      <c r="D17">
+        <v>8</v>
+      </c>
+      <c r="E17">
+        <v>13</v>
+      </c>
+      <c r="F17">
+        <v>9.5</v>
+      </c>
+      <c r="G17" t="s">
+        <v>2935</v>
+      </c>
+      <c r="H17" t="s">
+        <v>2936</v>
+      </c>
+      <c r="I17" t="s">
+        <v>2937</v>
+      </c>
+      <c r="J17" t="s">
+        <v>2938</v>
+      </c>
+      <c r="K17">
+        <v>620</v>
+      </c>
+      <c r="L17" t="s">
+        <v>1020</v>
+      </c>
+      <c r="M17">
+        <v>2</v>
+      </c>
+      <c r="N17">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -82692,7 +82800,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDB0DF-5C8E-46E0-A66A-0B4AF86ECDFD}">
   <dimension ref="A1:N167"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
5챕터 0.75 오버라이딩 => 0.9 디폴트 => 0.85 (재수정) 6챕터 0.7 => 제거 => 0.8 (재수정) 7챕터 0.8 => 제거
</commit_message>
<xml_diff>
--- a/Excel/Stage.xlsx
+++ b/Excel/Stage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectNoname\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0167D35-DAD1-40E4-8335-996E973C7467}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{409FC209-37AA-4774-ADED-75138D680E13}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{566BA174-F383-48D7-A97F-7F70BBC36EC1}"/>
   </bookViews>
@@ -46227,10 +46227,10 @@
         <v>1</v>
       </c>
       <c r="C701">
-        <v>572</v>
+        <v>541</v>
       </c>
       <c r="D701">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="E701" t="s">
         <v>1692</v>
@@ -46283,10 +46283,10 @@
         <v>2</v>
       </c>
       <c r="C702">
-        <v>572</v>
+        <v>541</v>
       </c>
       <c r="D702">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="I702" t="b">
         <v>1</v>
@@ -46330,10 +46330,10 @@
         <v>3</v>
       </c>
       <c r="C703">
-        <v>572</v>
+        <v>541</v>
       </c>
       <c r="D703">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="I703" t="b">
         <v>1</v>
@@ -46377,10 +46377,10 @@
         <v>4</v>
       </c>
       <c r="C704">
-        <v>572</v>
+        <v>541</v>
       </c>
       <c r="D704">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="I704" t="b">
         <v>1</v>
@@ -46424,10 +46424,10 @@
         <v>5</v>
       </c>
       <c r="C705">
-        <v>572</v>
+        <v>541</v>
       </c>
       <c r="D705">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="I705" t="b">
         <v>1</v>
@@ -46471,10 +46471,10 @@
         <v>6</v>
       </c>
       <c r="C706">
-        <v>687</v>
+        <v>649</v>
       </c>
       <c r="D706">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="I706" t="b">
         <v>1</v>
@@ -46518,10 +46518,10 @@
         <v>7</v>
       </c>
       <c r="C707">
-        <v>687</v>
+        <v>649</v>
       </c>
       <c r="D707">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="I707" t="b">
         <v>1</v>
@@ -46565,10 +46565,10 @@
         <v>8</v>
       </c>
       <c r="C708">
-        <v>687</v>
+        <v>649</v>
       </c>
       <c r="D708">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="I708" t="b">
         <v>1</v>
@@ -46612,10 +46612,10 @@
         <v>9</v>
       </c>
       <c r="C709">
-        <v>687</v>
+        <v>649</v>
       </c>
       <c r="D709">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="I709" t="b">
         <v>1</v>
@@ -46659,10 +46659,10 @@
         <v>10</v>
       </c>
       <c r="C710">
-        <v>687</v>
+        <v>649</v>
       </c>
       <c r="D710">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="I710" t="b">
         <v>1</v>
@@ -46709,10 +46709,10 @@
         <v>11</v>
       </c>
       <c r="C711">
-        <v>687</v>
+        <v>649</v>
       </c>
       <c r="D711">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="E711" t="s">
         <v>966</v>
@@ -46765,10 +46765,10 @@
         <v>12</v>
       </c>
       <c r="C712">
-        <v>687</v>
+        <v>649</v>
       </c>
       <c r="D712">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="I712" t="b">
         <v>1</v>
@@ -46812,10 +46812,10 @@
         <v>13</v>
       </c>
       <c r="C713">
-        <v>687</v>
+        <v>649</v>
       </c>
       <c r="D713">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="I713" t="b">
         <v>1</v>
@@ -46859,10 +46859,10 @@
         <v>14</v>
       </c>
       <c r="C714">
-        <v>687</v>
+        <v>649</v>
       </c>
       <c r="D714">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="I714" t="b">
         <v>1</v>
@@ -46906,10 +46906,10 @@
         <v>15</v>
       </c>
       <c r="C715">
-        <v>687</v>
+        <v>649</v>
       </c>
       <c r="D715">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="I715" t="b">
         <v>1</v>
@@ -46953,10 +46953,10 @@
         <v>16</v>
       </c>
       <c r="C716">
-        <v>801</v>
+        <v>757</v>
       </c>
       <c r="D716">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="I716" t="b">
         <v>1</v>
@@ -47000,10 +47000,10 @@
         <v>17</v>
       </c>
       <c r="C717">
-        <v>801</v>
+        <v>757</v>
       </c>
       <c r="D717">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="I717" t="b">
         <v>1</v>
@@ -47047,10 +47047,10 @@
         <v>18</v>
       </c>
       <c r="C718">
-        <v>801</v>
+        <v>757</v>
       </c>
       <c r="D718">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="I718" t="b">
         <v>1</v>
@@ -47094,10 +47094,10 @@
         <v>19</v>
       </c>
       <c r="C719">
-        <v>801</v>
+        <v>757</v>
       </c>
       <c r="D719">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="I719" t="b">
         <v>1</v>
@@ -47141,10 +47141,10 @@
         <v>20</v>
       </c>
       <c r="C720">
-        <v>801</v>
+        <v>757</v>
       </c>
       <c r="D720">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="I720" t="b">
         <v>1</v>
@@ -47191,10 +47191,10 @@
         <v>21</v>
       </c>
       <c r="C721">
-        <v>801</v>
+        <v>757</v>
       </c>
       <c r="D721">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="I721" t="b">
         <v>1</v>
@@ -47244,10 +47244,10 @@
         <v>22</v>
       </c>
       <c r="C722">
-        <v>801</v>
+        <v>757</v>
       </c>
       <c r="D722">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="I722" t="b">
         <v>1</v>
@@ -47291,10 +47291,10 @@
         <v>23</v>
       </c>
       <c r="C723">
-        <v>801</v>
+        <v>757</v>
       </c>
       <c r="D723">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="I723" t="b">
         <v>1</v>
@@ -47338,10 +47338,10 @@
         <v>24</v>
       </c>
       <c r="C724">
-        <v>801</v>
+        <v>757</v>
       </c>
       <c r="D724">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="I724" t="b">
         <v>1</v>
@@ -47385,10 +47385,10 @@
         <v>25</v>
       </c>
       <c r="C725">
-        <v>801</v>
+        <v>757</v>
       </c>
       <c r="D725">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="I725" t="b">
         <v>1</v>
@@ -47432,10 +47432,10 @@
         <v>26</v>
       </c>
       <c r="C726">
-        <v>916</v>
+        <v>865</v>
       </c>
       <c r="D726">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="I726" t="b">
         <v>1</v>
@@ -47479,10 +47479,10 @@
         <v>27</v>
       </c>
       <c r="C727">
-        <v>916</v>
+        <v>865</v>
       </c>
       <c r="D727">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="I727" t="b">
         <v>1</v>
@@ -47526,10 +47526,10 @@
         <v>28</v>
       </c>
       <c r="C728">
-        <v>916</v>
+        <v>865</v>
       </c>
       <c r="D728">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="I728" t="b">
         <v>1</v>
@@ -47573,10 +47573,10 @@
         <v>29</v>
       </c>
       <c r="C729">
-        <v>916</v>
+        <v>865</v>
       </c>
       <c r="D729">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="I729" t="b">
         <v>1</v>
@@ -47620,10 +47620,10 @@
         <v>30</v>
       </c>
       <c r="C730">
-        <v>916</v>
+        <v>865</v>
       </c>
       <c r="D730">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="I730" t="b">
         <v>1</v>
@@ -47670,10 +47670,10 @@
         <v>31</v>
       </c>
       <c r="C731">
-        <v>916</v>
+        <v>865</v>
       </c>
       <c r="D731">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="E731" t="s">
         <v>1788</v>
@@ -47726,10 +47726,10 @@
         <v>32</v>
       </c>
       <c r="C732">
-        <v>916</v>
+        <v>865</v>
       </c>
       <c r="D732">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="I732" t="b">
         <v>1</v>
@@ -47773,10 +47773,10 @@
         <v>33</v>
       </c>
       <c r="C733">
-        <v>916</v>
+        <v>865</v>
       </c>
       <c r="D733">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="I733" t="b">
         <v>1</v>
@@ -47820,10 +47820,10 @@
         <v>34</v>
       </c>
       <c r="C734">
-        <v>916</v>
+        <v>865</v>
       </c>
       <c r="D734">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="I734" t="b">
         <v>1</v>
@@ -47867,10 +47867,10 @@
         <v>35</v>
       </c>
       <c r="C735">
-        <v>916</v>
+        <v>865</v>
       </c>
       <c r="D735">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="I735" t="b">
         <v>1</v>
@@ -47914,10 +47914,10 @@
         <v>36</v>
       </c>
       <c r="C736">
-        <v>1030</v>
+        <v>973</v>
       </c>
       <c r="D736">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="I736" t="b">
         <v>1</v>
@@ -47961,10 +47961,10 @@
         <v>37</v>
       </c>
       <c r="C737">
-        <v>1030</v>
+        <v>973</v>
       </c>
       <c r="D737">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="I737" t="b">
         <v>1</v>
@@ -48008,10 +48008,10 @@
         <v>38</v>
       </c>
       <c r="C738">
-        <v>1030</v>
+        <v>973</v>
       </c>
       <c r="D738">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="I738" t="b">
         <v>1</v>
@@ -48055,10 +48055,10 @@
         <v>39</v>
       </c>
       <c r="C739">
-        <v>1030</v>
+        <v>973</v>
       </c>
       <c r="D739">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="I739" t="b">
         <v>1</v>
@@ -48102,10 +48102,10 @@
         <v>40</v>
       </c>
       <c r="C740">
-        <v>1030</v>
+        <v>973</v>
       </c>
       <c r="D740">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="I740" t="b">
         <v>1</v>
@@ -48152,10 +48152,10 @@
         <v>41</v>
       </c>
       <c r="C741">
-        <v>1030</v>
+        <v>973</v>
       </c>
       <c r="D741">
-        <v>222</v>
+        <v>210</v>
       </c>
       <c r="I741" t="b">
         <v>1</v>
@@ -48205,10 +48205,10 @@
         <v>42</v>
       </c>
       <c r="C742">
-        <v>1030</v>
+        <v>973</v>
       </c>
       <c r="D742">
-        <v>222</v>
+        <v>210</v>
       </c>
       <c r="I742" t="b">
         <v>1</v>
@@ -48252,10 +48252,10 @@
         <v>43</v>
       </c>
       <c r="C743">
-        <v>1030</v>
+        <v>973</v>
       </c>
       <c r="D743">
-        <v>222</v>
+        <v>210</v>
       </c>
       <c r="I743" t="b">
         <v>1</v>
@@ -48299,10 +48299,10 @@
         <v>44</v>
       </c>
       <c r="C744">
-        <v>1030</v>
+        <v>973</v>
       </c>
       <c r="D744">
-        <v>222</v>
+        <v>210</v>
       </c>
       <c r="I744" t="b">
         <v>1</v>
@@ -48346,10 +48346,10 @@
         <v>45</v>
       </c>
       <c r="C745">
-        <v>1030</v>
+        <v>973</v>
       </c>
       <c r="D745">
-        <v>222</v>
+        <v>210</v>
       </c>
       <c r="I745" t="b">
         <v>1</v>
@@ -48393,10 +48393,10 @@
         <v>46</v>
       </c>
       <c r="C746">
-        <v>1145</v>
+        <v>1081</v>
       </c>
       <c r="D746">
-        <v>222</v>
+        <v>210</v>
       </c>
       <c r="I746" t="b">
         <v>1</v>
@@ -48440,10 +48440,10 @@
         <v>47</v>
       </c>
       <c r="C747">
-        <v>1145</v>
+        <v>1081</v>
       </c>
       <c r="D747">
-        <v>222</v>
+        <v>210</v>
       </c>
       <c r="I747" t="b">
         <v>1</v>
@@ -48487,10 +48487,10 @@
         <v>48</v>
       </c>
       <c r="C748">
-        <v>1145</v>
+        <v>1081</v>
       </c>
       <c r="D748">
-        <v>222</v>
+        <v>210</v>
       </c>
       <c r="I748" t="b">
         <v>1</v>
@@ -48534,10 +48534,10 @@
         <v>49</v>
       </c>
       <c r="C749">
-        <v>1145</v>
+        <v>1081</v>
       </c>
       <c r="D749">
-        <v>222</v>
+        <v>210</v>
       </c>
       <c r="I749" t="b">
         <v>1</v>
@@ -48581,10 +48581,10 @@
         <v>50</v>
       </c>
       <c r="C750">
-        <v>1488</v>
+        <v>1406</v>
       </c>
       <c r="D750">
-        <v>222</v>
+        <v>210</v>
       </c>
       <c r="I750" t="b">
         <v>1</v>
@@ -48631,10 +48631,10 @@
         <v>1</v>
       </c>
       <c r="C751">
-        <v>1032</v>
+        <v>917</v>
       </c>
       <c r="D751">
-        <v>276</v>
+        <v>245</v>
       </c>
       <c r="E751" t="s">
         <v>2050</v>
@@ -48687,10 +48687,10 @@
         <v>2</v>
       </c>
       <c r="C752">
-        <v>1032</v>
+        <v>917</v>
       </c>
       <c r="D752">
-        <v>276</v>
+        <v>245</v>
       </c>
       <c r="I752" t="b">
         <v>1</v>
@@ -48734,10 +48734,10 @@
         <v>3</v>
       </c>
       <c r="C753">
-        <v>1032</v>
+        <v>917</v>
       </c>
       <c r="D753">
-        <v>276</v>
+        <v>245</v>
       </c>
       <c r="I753" t="b">
         <v>1</v>
@@ -48781,10 +48781,10 @@
         <v>4</v>
       </c>
       <c r="C754">
-        <v>1032</v>
+        <v>917</v>
       </c>
       <c r="D754">
-        <v>276</v>
+        <v>245</v>
       </c>
       <c r="I754" t="b">
         <v>1</v>
@@ -48828,10 +48828,10 @@
         <v>5</v>
       </c>
       <c r="C755">
-        <v>1032</v>
+        <v>917</v>
       </c>
       <c r="D755">
-        <v>276</v>
+        <v>245</v>
       </c>
       <c r="I755" t="b">
         <v>1</v>
@@ -48875,10 +48875,10 @@
         <v>6</v>
       </c>
       <c r="C756">
-        <v>1238</v>
+        <v>1101</v>
       </c>
       <c r="D756">
-        <v>276</v>
+        <v>245</v>
       </c>
       <c r="I756" t="b">
         <v>1</v>
@@ -48922,10 +48922,10 @@
         <v>7</v>
       </c>
       <c r="C757">
-        <v>1238</v>
+        <v>1101</v>
       </c>
       <c r="D757">
-        <v>276</v>
+        <v>245</v>
       </c>
       <c r="I757" t="b">
         <v>1</v>
@@ -48969,10 +48969,10 @@
         <v>8</v>
       </c>
       <c r="C758">
-        <v>1238</v>
+        <v>1101</v>
       </c>
       <c r="D758">
-        <v>276</v>
+        <v>245</v>
       </c>
       <c r="I758" t="b">
         <v>1</v>
@@ -49016,10 +49016,10 @@
         <v>9</v>
       </c>
       <c r="C759">
-        <v>1238</v>
+        <v>1101</v>
       </c>
       <c r="D759">
-        <v>276</v>
+        <v>245</v>
       </c>
       <c r="I759" t="b">
         <v>1</v>
@@ -49063,10 +49063,10 @@
         <v>10</v>
       </c>
       <c r="C760">
-        <v>1238</v>
+        <v>1101</v>
       </c>
       <c r="D760">
-        <v>276</v>
+        <v>245</v>
       </c>
       <c r="I760" t="b">
         <v>1</v>
@@ -49113,10 +49113,10 @@
         <v>11</v>
       </c>
       <c r="C761">
-        <v>1238</v>
+        <v>1101</v>
       </c>
       <c r="D761">
-        <v>296</v>
+        <v>263</v>
       </c>
       <c r="I761" t="b">
         <v>1</v>
@@ -49166,10 +49166,10 @@
         <v>12</v>
       </c>
       <c r="C762">
-        <v>1238</v>
+        <v>1101</v>
       </c>
       <c r="D762">
-        <v>296</v>
+        <v>263</v>
       </c>
       <c r="I762" t="b">
         <v>1</v>
@@ -49213,10 +49213,10 @@
         <v>13</v>
       </c>
       <c r="C763">
-        <v>1238</v>
+        <v>1101</v>
       </c>
       <c r="D763">
-        <v>296</v>
+        <v>263</v>
       </c>
       <c r="I763" t="b">
         <v>1</v>
@@ -49260,10 +49260,10 @@
         <v>14</v>
       </c>
       <c r="C764">
-        <v>1238</v>
+        <v>1101</v>
       </c>
       <c r="D764">
-        <v>296</v>
+        <v>263</v>
       </c>
       <c r="I764" t="b">
         <v>1</v>
@@ -49307,10 +49307,10 @@
         <v>15</v>
       </c>
       <c r="C765">
-        <v>1238</v>
+        <v>1101</v>
       </c>
       <c r="D765">
-        <v>296</v>
+        <v>263</v>
       </c>
       <c r="I765" t="b">
         <v>1</v>
@@ -49354,10 +49354,10 @@
         <v>16</v>
       </c>
       <c r="C766">
-        <v>1444</v>
+        <v>1284</v>
       </c>
       <c r="D766">
-        <v>296</v>
+        <v>263</v>
       </c>
       <c r="I766" t="b">
         <v>1</v>
@@ -49401,10 +49401,10 @@
         <v>17</v>
       </c>
       <c r="C767">
-        <v>1444</v>
+        <v>1284</v>
       </c>
       <c r="D767">
-        <v>296</v>
+        <v>263</v>
       </c>
       <c r="I767" t="b">
         <v>1</v>
@@ -49448,10 +49448,10 @@
         <v>18</v>
       </c>
       <c r="C768">
-        <v>1444</v>
+        <v>1284</v>
       </c>
       <c r="D768">
-        <v>296</v>
+        <v>263</v>
       </c>
       <c r="I768" t="b">
         <v>1</v>
@@ -49495,10 +49495,10 @@
         <v>19</v>
       </c>
       <c r="C769">
-        <v>1444</v>
+        <v>1284</v>
       </c>
       <c r="D769">
-        <v>296</v>
+        <v>263</v>
       </c>
       <c r="I769" t="b">
         <v>1</v>
@@ -49542,10 +49542,10 @@
         <v>20</v>
       </c>
       <c r="C770">
-        <v>1444</v>
+        <v>1284</v>
       </c>
       <c r="D770">
-        <v>296</v>
+        <v>263</v>
       </c>
       <c r="I770" t="b">
         <v>1</v>
@@ -49592,10 +49592,10 @@
         <v>21</v>
       </c>
       <c r="C771">
-        <v>1444</v>
+        <v>1284</v>
       </c>
       <c r="D771">
-        <v>317</v>
+        <v>282</v>
       </c>
       <c r="E771" t="s">
         <v>1789</v>
@@ -49648,10 +49648,10 @@
         <v>22</v>
       </c>
       <c r="C772">
-        <v>1444</v>
+        <v>1284</v>
       </c>
       <c r="D772">
-        <v>317</v>
+        <v>282</v>
       </c>
       <c r="I772" t="b">
         <v>1</v>
@@ -49695,10 +49695,10 @@
         <v>23</v>
       </c>
       <c r="C773">
-        <v>1444</v>
+        <v>1284</v>
       </c>
       <c r="D773">
-        <v>317</v>
+        <v>282</v>
       </c>
       <c r="I773" t="b">
         <v>1</v>
@@ -49742,10 +49742,10 @@
         <v>24</v>
       </c>
       <c r="C774">
-        <v>1444</v>
+        <v>1284</v>
       </c>
       <c r="D774">
-        <v>317</v>
+        <v>282</v>
       </c>
       <c r="I774" t="b">
         <v>1</v>
@@ -49789,10 +49789,10 @@
         <v>25</v>
       </c>
       <c r="C775">
-        <v>1444</v>
+        <v>1284</v>
       </c>
       <c r="D775">
-        <v>317</v>
+        <v>282</v>
       </c>
       <c r="I775" t="b">
         <v>1</v>
@@ -49836,10 +49836,10 @@
         <v>26</v>
       </c>
       <c r="C776">
-        <v>1651</v>
+        <v>1467</v>
       </c>
       <c r="D776">
-        <v>317</v>
+        <v>282</v>
       </c>
       <c r="I776" t="b">
         <v>1</v>
@@ -49883,10 +49883,10 @@
         <v>27</v>
       </c>
       <c r="C777">
-        <v>1651</v>
+        <v>1467</v>
       </c>
       <c r="D777">
-        <v>317</v>
+        <v>282</v>
       </c>
       <c r="I777" t="b">
         <v>1</v>
@@ -49930,10 +49930,10 @@
         <v>28</v>
       </c>
       <c r="C778">
-        <v>1651</v>
+        <v>1467</v>
       </c>
       <c r="D778">
-        <v>317</v>
+        <v>282</v>
       </c>
       <c r="I778" t="b">
         <v>1</v>
@@ -49977,10 +49977,10 @@
         <v>29</v>
       </c>
       <c r="C779">
-        <v>1651</v>
+        <v>1467</v>
       </c>
       <c r="D779">
-        <v>317</v>
+        <v>282</v>
       </c>
       <c r="I779" t="b">
         <v>1</v>
@@ -50024,10 +50024,10 @@
         <v>30</v>
       </c>
       <c r="C780">
-        <v>1651</v>
+        <v>1467</v>
       </c>
       <c r="D780">
-        <v>317</v>
+        <v>282</v>
       </c>
       <c r="I780" t="b">
         <v>1</v>
@@ -50074,10 +50074,10 @@
         <v>31</v>
       </c>
       <c r="C781">
-        <v>1651</v>
+        <v>1467</v>
       </c>
       <c r="D781">
-        <v>338</v>
+        <v>300</v>
       </c>
       <c r="I781" t="b">
         <v>1</v>
@@ -50127,10 +50127,10 @@
         <v>32</v>
       </c>
       <c r="C782">
-        <v>1651</v>
+        <v>1467</v>
       </c>
       <c r="D782">
-        <v>338</v>
+        <v>300</v>
       </c>
       <c r="I782" t="b">
         <v>1</v>
@@ -50174,10 +50174,10 @@
         <v>33</v>
       </c>
       <c r="C783">
-        <v>1651</v>
+        <v>1467</v>
       </c>
       <c r="D783">
-        <v>338</v>
+        <v>300</v>
       </c>
       <c r="I783" t="b">
         <v>1</v>
@@ -50221,10 +50221,10 @@
         <v>34</v>
       </c>
       <c r="C784">
-        <v>1651</v>
+        <v>1467</v>
       </c>
       <c r="D784">
-        <v>338</v>
+        <v>300</v>
       </c>
       <c r="I784" t="b">
         <v>1</v>
@@ -50268,10 +50268,10 @@
         <v>35</v>
       </c>
       <c r="C785">
-        <v>1651</v>
+        <v>1467</v>
       </c>
       <c r="D785">
-        <v>338</v>
+        <v>300</v>
       </c>
       <c r="I785" t="b">
         <v>1</v>
@@ -50315,10 +50315,10 @@
         <v>36</v>
       </c>
       <c r="C786">
-        <v>1857</v>
+        <v>1651</v>
       </c>
       <c r="D786">
-        <v>338</v>
+        <v>300</v>
       </c>
       <c r="I786" t="b">
         <v>1</v>
@@ -50362,10 +50362,10 @@
         <v>37</v>
       </c>
       <c r="C787">
-        <v>1857</v>
+        <v>1651</v>
       </c>
       <c r="D787">
-        <v>338</v>
+        <v>300</v>
       </c>
       <c r="I787" t="b">
         <v>1</v>
@@ -50409,10 +50409,10 @@
         <v>38</v>
       </c>
       <c r="C788">
-        <v>1857</v>
+        <v>1651</v>
       </c>
       <c r="D788">
-        <v>338</v>
+        <v>300</v>
       </c>
       <c r="I788" t="b">
         <v>1</v>
@@ -50456,10 +50456,10 @@
         <v>39</v>
       </c>
       <c r="C789">
-        <v>1857</v>
+        <v>1651</v>
       </c>
       <c r="D789">
-        <v>338</v>
+        <v>300</v>
       </c>
       <c r="I789" t="b">
         <v>1</v>
@@ -50503,10 +50503,10 @@
         <v>40</v>
       </c>
       <c r="C790">
-        <v>1857</v>
+        <v>1651</v>
       </c>
       <c r="D790">
-        <v>338</v>
+        <v>300</v>
       </c>
       <c r="I790" t="b">
         <v>1</v>
@@ -50553,10 +50553,10 @@
         <v>41</v>
       </c>
       <c r="C791">
-        <v>1857</v>
+        <v>1651</v>
       </c>
       <c r="D791">
-        <v>358</v>
+        <v>318</v>
       </c>
       <c r="E791" t="s">
         <v>1477</v>
@@ -50609,10 +50609,10 @@
         <v>42</v>
       </c>
       <c r="C792">
-        <v>1857</v>
+        <v>1651</v>
       </c>
       <c r="D792">
-        <v>358</v>
+        <v>318</v>
       </c>
       <c r="I792" t="b">
         <v>1</v>
@@ -50656,10 +50656,10 @@
         <v>43</v>
       </c>
       <c r="C793">
-        <v>1857</v>
+        <v>1651</v>
       </c>
       <c r="D793">
-        <v>358</v>
+        <v>318</v>
       </c>
       <c r="I793" t="b">
         <v>1</v>
@@ -50703,10 +50703,10 @@
         <v>44</v>
       </c>
       <c r="C794">
-        <v>1857</v>
+        <v>1651</v>
       </c>
       <c r="D794">
-        <v>358</v>
+        <v>318</v>
       </c>
       <c r="I794" t="b">
         <v>1</v>
@@ -50750,10 +50750,10 @@
         <v>45</v>
       </c>
       <c r="C795">
-        <v>1857</v>
+        <v>1651</v>
       </c>
       <c r="D795">
-        <v>358</v>
+        <v>318</v>
       </c>
       <c r="I795" t="b">
         <v>1</v>
@@ -50797,10 +50797,10 @@
         <v>46</v>
       </c>
       <c r="C796">
-        <v>2063</v>
+        <v>1834</v>
       </c>
       <c r="D796">
-        <v>358</v>
+        <v>318</v>
       </c>
       <c r="I796" t="b">
         <v>1</v>
@@ -50844,10 +50844,10 @@
         <v>47</v>
       </c>
       <c r="C797">
-        <v>2063</v>
+        <v>1834</v>
       </c>
       <c r="D797">
-        <v>358</v>
+        <v>318</v>
       </c>
       <c r="I797" t="b">
         <v>1</v>
@@ -50891,10 +50891,10 @@
         <v>48</v>
       </c>
       <c r="C798">
-        <v>2063</v>
+        <v>1834</v>
       </c>
       <c r="D798">
-        <v>358</v>
+        <v>318</v>
       </c>
       <c r="I798" t="b">
         <v>1</v>
@@ -50938,10 +50938,10 @@
         <v>49</v>
       </c>
       <c r="C799">
-        <v>2063</v>
+        <v>1834</v>
       </c>
       <c r="D799">
-        <v>358</v>
+        <v>318</v>
       </c>
       <c r="I799" t="b">
         <v>1</v>
@@ -50985,10 +50985,10 @@
         <v>50</v>
       </c>
       <c r="C800">
-        <v>2682</v>
+        <v>2384</v>
       </c>
       <c r="D800">
-        <v>358</v>
+        <v>318</v>
       </c>
       <c r="I800" t="b">
         <v>1</v>

</xml_diff>